<commit_message>
fix locale $ add btn
</commit_message>
<xml_diff>
--- a/locale/888tron_locale.xlsx
+++ b/locale/888tron_locale.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF67D82C-6E23-475E-80A2-74FA9FB28CE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79678579-418F-447E-B642-FD933CF51406}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="1136">
   <si>
     <t>fairness</t>
   </si>
@@ -5878,13 +5878,37 @@
     <t>888 바이백 풀</t>
   </si>
   <si>
-    <t>팀 수입의 15%는 향후 3개월 동안 888 토큰을 다시 사는데 쓰인다.</t>
-  </si>
-  <si>
     <t>888토큰 소각</t>
   </si>
   <si>
     <t>4월 9일부터 2주마다 바이백 풀에 쌓인 888토큰의 20%가 소각 될 것이다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">팀 수입의 15%는 향후 3개월 동안 888 토큰을 다시 구매하는데 쓰인다. </t>
+  </si>
+  <si>
+    <t>buy_trx</t>
+  </si>
+  <si>
+    <t>Buy TRX</t>
+  </si>
+  <si>
+    <t>Kaufen TRX</t>
+  </si>
+  <si>
+    <t>Купить TRX</t>
+  </si>
+  <si>
+    <t>사다 TRX</t>
+  </si>
+  <si>
+    <t>購買 TRX</t>
+  </si>
+  <si>
+    <t>Comprar TRX</t>
+  </si>
+  <si>
+    <t>Almak TRX</t>
   </si>
 </sst>
 </file>
@@ -6392,10 +6416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
     <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+      <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -7651,6 +7675,14 @@
         <v>1120</v>
       </c>
     </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1129</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7659,10 +7691,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E6A467-D0AF-459C-BE00-51F2B53B650E}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
     <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+      <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8918,6 +8950,14 @@
         <v>1120</v>
       </c>
     </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8925,10 +8965,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
     <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:XFD156"/>
+      <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -10185,6 +10225,14 @@
         <v>1122</v>
       </c>
     </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10193,10 +10241,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147:B150"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -11385,7 +11433,7 @@
         <v>1073</v>
       </c>
       <c r="B148" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -11393,7 +11441,7 @@
         <v>1066</v>
       </c>
       <c r="B149" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -11401,7 +11449,7 @@
         <v>1068</v>
       </c>
       <c r="B150" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -11450,6 +11498,14 @@
       </c>
       <c r="B156" t="s">
         <v>1121</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1132</v>
       </c>
     </row>
   </sheetData>
@@ -11460,10 +11516,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:XFD156"/>
+      <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -12719,6 +12775,14 @@
         <v>1123</v>
       </c>
     </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1133</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12727,10 +12791,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
     <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+      <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -13986,6 +14050,14 @@
         <v>1120</v>
       </c>
     </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13994,10 +14066,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:XFD156"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -15253,6 +15325,14 @@
         <v>1120</v>
       </c>
     </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix css & ch locale
</commit_message>
<xml_diff>
--- a/locale/888tron_locale.xlsx
+++ b/locale/888tron_locale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\FIRE\tronGamesClient\locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549CC6EF-9CB1-4742-931F-B1BE44D517BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21CFD32-D54D-4CE5-8912-435DBDBB2B1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="993" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -10614,9 +10614,6 @@
     </r>
   </si>
   <si>
-    <t>ゲーム</t>
-  </si>
-  <si>
     <t>Juego limpio</t>
   </si>
   <si>
@@ -11557,6 +11554,9 @@
   </si>
   <si>
     <t>Маленькие ставки (50-100 ТРХ) потребляют такую же энергию как и большие (~0,5 TRX), но приносят меньше токенов и доход.</t>
+  </si>
+  <si>
+    <t>游戏</t>
   </si>
 </sst>
 </file>
@@ -13371,50 +13371,50 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B160" t="s">
         <v>1140</v>
-      </c>
-      <c r="B160" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B161" t="s">
         <v>1142</v>
-      </c>
-      <c r="B161" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B162" t="s">
         <v>1144</v>
-      </c>
-      <c r="B162" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B163" t="s">
         <v>1146</v>
-      </c>
-      <c r="B163" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B164" t="s">
         <v>1157</v>
-      </c>
-      <c r="B164" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B165" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>
@@ -14711,50 +14711,50 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B160" t="s">
         <v>1140</v>
-      </c>
-      <c r="B160" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B161" t="s">
         <v>1142</v>
-      </c>
-      <c r="B161" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B162" t="s">
         <v>1144</v>
-      </c>
-      <c r="B162" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B163" t="s">
         <v>1146</v>
-      </c>
-      <c r="B163" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B164" t="s">
         <v>1157</v>
-      </c>
-      <c r="B164" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B165" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>
@@ -15550,7 +15550,7 @@
         <v>187</v>
       </c>
       <c r="B97" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -16051,50 +16051,50 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B160" t="s">
         <v>1140</v>
-      </c>
-      <c r="B160" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B161" t="s">
         <v>1142</v>
-      </c>
-      <c r="B161" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B162" t="s">
         <v>1144</v>
-      </c>
-      <c r="B162" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B163" t="s">
         <v>1146</v>
-      </c>
-      <c r="B163" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B164" t="s">
         <v>1157</v>
-      </c>
-      <c r="B164" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B165" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>
@@ -17338,7 +17338,7 @@
         <v>296</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -17391,50 +17391,50 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B160" t="s">
         <v>1140</v>
-      </c>
-      <c r="B160" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B161" t="s">
         <v>1142</v>
-      </c>
-      <c r="B161" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B162" t="s">
         <v>1144</v>
-      </c>
-      <c r="B162" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B163" t="s">
         <v>1146</v>
-      </c>
-      <c r="B163" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B164" t="s">
         <v>1157</v>
-      </c>
-      <c r="B164" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B165" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>
@@ -17447,8 +17447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A165" sqref="A1:B165"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17622,7 +17622,7 @@
         <v>40</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -17798,7 +17798,7 @@
         <v>84</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -17806,7 +17806,7 @@
         <v>86</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -17878,7 +17878,7 @@
         <v>103</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -17886,7 +17886,7 @@
         <v>105</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -17894,7 +17894,7 @@
         <v>107</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -18126,7 +18126,7 @@
         <v>161</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -18142,7 +18142,7 @@
         <v>165</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -18158,7 +18158,7 @@
         <v>169</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -18166,7 +18166,7 @@
         <v>171</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -18718,7 +18718,7 @@
         <v>308</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>857</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -18726,55 +18726,55 @@
         <v>306</v>
       </c>
       <c r="B159" s="12" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B161" s="12" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B162" s="12" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B164" s="12" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B165" s="12" t="s">
         <v>1161</v>
-      </c>
-      <c r="B165" s="12" t="s">
-        <v>1162</v>
       </c>
     </row>
   </sheetData>
@@ -18802,7 +18802,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -18810,7 +18810,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -18818,7 +18818,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -18826,7 +18826,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -18834,7 +18834,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -18842,7 +18842,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -18850,7 +18850,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -18858,7 +18858,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -18874,7 +18874,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -18882,7 +18882,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -18890,7 +18890,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -18898,7 +18898,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -18906,7 +18906,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -18914,7 +18914,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -18922,7 +18922,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -18930,7 +18930,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -18938,7 +18938,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -18946,7 +18946,7 @@
         <v>36</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -18954,7 +18954,7 @@
         <v>38</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -18962,7 +18962,7 @@
         <v>40</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -18970,7 +18970,7 @@
         <v>42</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -18978,7 +18978,7 @@
         <v>44</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -18986,7 +18986,7 @@
         <v>46</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -18994,7 +18994,7 @@
         <v>48</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -19002,7 +19002,7 @@
         <v>50</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -19010,7 +19010,7 @@
         <v>52</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -19018,7 +19018,7 @@
         <v>54</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -19026,7 +19026,7 @@
         <v>56</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -19034,7 +19034,7 @@
         <v>58</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -19042,7 +19042,7 @@
         <v>60</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -19050,7 +19050,7 @@
         <v>62</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -19058,7 +19058,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -19122,7 +19122,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -19146,7 +19146,7 @@
         <v>86</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -19154,7 +19154,7 @@
         <v>88</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -19162,7 +19162,7 @@
         <v>89</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -19170,7 +19170,7 @@
         <v>91</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -19178,7 +19178,7 @@
         <v>93</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -19186,7 +19186,7 @@
         <v>95</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -19194,15 +19194,15 @@
         <v>97</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="9" t="s">
+        <v>897</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>898</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -19210,7 +19210,7 @@
         <v>101</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -19218,7 +19218,7 @@
         <v>103</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -19226,7 +19226,7 @@
         <v>105</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -19234,7 +19234,7 @@
         <v>107</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -19242,7 +19242,7 @@
         <v>109</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -19250,7 +19250,7 @@
         <v>111</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -19258,7 +19258,7 @@
         <v>113</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -19266,7 +19266,7 @@
         <v>115</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -19274,7 +19274,7 @@
         <v>117</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -19282,7 +19282,7 @@
         <v>119</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -19290,7 +19290,7 @@
         <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -19298,7 +19298,7 @@
         <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -19306,7 +19306,7 @@
         <v>125</v>
       </c>
       <c r="B64" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -19314,7 +19314,7 @@
         <v>127</v>
       </c>
       <c r="B65" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -19322,7 +19322,7 @@
         <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -19330,7 +19330,7 @@
         <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -19338,7 +19338,7 @@
         <v>133</v>
       </c>
       <c r="B68" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -19346,7 +19346,7 @@
         <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -19354,7 +19354,7 @@
         <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -19362,7 +19362,7 @@
         <v>139</v>
       </c>
       <c r="B71" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -19370,7 +19370,7 @@
         <v>141</v>
       </c>
       <c r="B72" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -19378,7 +19378,7 @@
         <v>143</v>
       </c>
       <c r="B73" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -19386,7 +19386,7 @@
         <v>145</v>
       </c>
       <c r="B74" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -19402,7 +19402,7 @@
         <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -19410,7 +19410,7 @@
         <v>151</v>
       </c>
       <c r="B77" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -19418,7 +19418,7 @@
         <v>153</v>
       </c>
       <c r="B78" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -19426,7 +19426,7 @@
         <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -19434,7 +19434,7 @@
         <v>157</v>
       </c>
       <c r="B80" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -19450,7 +19450,7 @@
         <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -19458,7 +19458,7 @@
         <v>24</v>
       </c>
       <c r="B83" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -19466,7 +19466,7 @@
         <v>161</v>
       </c>
       <c r="B84" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -19474,7 +19474,7 @@
         <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -19482,7 +19482,7 @@
         <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -19490,7 +19490,7 @@
         <v>167</v>
       </c>
       <c r="B87" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -19498,7 +19498,7 @@
         <v>169</v>
       </c>
       <c r="B88" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -19506,7 +19506,7 @@
         <v>171</v>
       </c>
       <c r="B89" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -19514,7 +19514,7 @@
         <v>173</v>
       </c>
       <c r="B90" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -19522,7 +19522,7 @@
         <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -19538,7 +19538,7 @@
         <v>179</v>
       </c>
       <c r="B93" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -19546,7 +19546,7 @@
         <v>181</v>
       </c>
       <c r="B94" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -19554,7 +19554,7 @@
         <v>183</v>
       </c>
       <c r="B95" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -19562,7 +19562,7 @@
         <v>185</v>
       </c>
       <c r="B96" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -19570,7 +19570,7 @@
         <v>187</v>
       </c>
       <c r="B97" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -19578,7 +19578,7 @@
         <v>189</v>
       </c>
       <c r="B98" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -19586,7 +19586,7 @@
         <v>191</v>
       </c>
       <c r="B99" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -19602,7 +19602,7 @@
         <v>195</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -19610,7 +19610,7 @@
         <v>197</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -19618,7 +19618,7 @@
         <v>199</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -19626,7 +19626,7 @@
         <v>201</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -19634,7 +19634,7 @@
         <v>202</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -19642,7 +19642,7 @@
         <v>204</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -19650,7 +19650,7 @@
         <v>206</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -19658,7 +19658,7 @@
         <v>208</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -19666,7 +19666,7 @@
         <v>209</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -19674,7 +19674,7 @@
         <v>211</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -19682,7 +19682,7 @@
         <v>213</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -19690,7 +19690,7 @@
         <v>215</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -19698,7 +19698,7 @@
         <v>216</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -19706,7 +19706,7 @@
         <v>218</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -19714,7 +19714,7 @@
         <v>220</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -19722,7 +19722,7 @@
         <v>222</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -19730,7 +19730,7 @@
         <v>224</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -19738,7 +19738,7 @@
         <v>226</v>
       </c>
       <c r="B118" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -19746,7 +19746,7 @@
         <v>228</v>
       </c>
       <c r="B119" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -19754,7 +19754,7 @@
         <v>230</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -19762,7 +19762,7 @@
         <v>232</v>
       </c>
       <c r="B121" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -19770,7 +19770,7 @@
         <v>234</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -19778,7 +19778,7 @@
         <v>236</v>
       </c>
       <c r="B123" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -19786,7 +19786,7 @@
         <v>238</v>
       </c>
       <c r="B124" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -19794,7 +19794,7 @@
         <v>240</v>
       </c>
       <c r="B125" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -19802,7 +19802,7 @@
         <v>242</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -19810,7 +19810,7 @@
         <v>244</v>
       </c>
       <c r="B127" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -19818,7 +19818,7 @@
         <v>246</v>
       </c>
       <c r="B128" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -19826,7 +19826,7 @@
         <v>248</v>
       </c>
       <c r="B129" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -19834,7 +19834,7 @@
         <v>250</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -19842,7 +19842,7 @@
         <v>252</v>
       </c>
       <c r="B131" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -19850,7 +19850,7 @@
         <v>254</v>
       </c>
       <c r="B132" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -19858,7 +19858,7 @@
         <v>256</v>
       </c>
       <c r="B133" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -19866,7 +19866,7 @@
         <v>258</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -19874,7 +19874,7 @@
         <v>260</v>
       </c>
       <c r="B135" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -19882,7 +19882,7 @@
         <v>262</v>
       </c>
       <c r="B136" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -19890,7 +19890,7 @@
         <v>264</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -19898,7 +19898,7 @@
         <v>266</v>
       </c>
       <c r="B138" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -19906,7 +19906,7 @@
         <v>268</v>
       </c>
       <c r="B139" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -19914,7 +19914,7 @@
         <v>270</v>
       </c>
       <c r="B140" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -19922,7 +19922,7 @@
         <v>272</v>
       </c>
       <c r="B141" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -19930,7 +19930,7 @@
         <v>274</v>
       </c>
       <c r="B142" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -19938,7 +19938,7 @@
         <v>276</v>
       </c>
       <c r="B143" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -19962,7 +19962,7 @@
         <v>282</v>
       </c>
       <c r="B146" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -19970,7 +19970,7 @@
         <v>284</v>
       </c>
       <c r="B147" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -19978,7 +19978,7 @@
         <v>286</v>
       </c>
       <c r="B148" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -19986,7 +19986,7 @@
         <v>288</v>
       </c>
       <c r="B149" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -19994,7 +19994,7 @@
         <v>290</v>
       </c>
       <c r="B150" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -20002,7 +20002,7 @@
         <v>292</v>
       </c>
       <c r="B151" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -20010,7 +20010,7 @@
         <v>294</v>
       </c>
       <c r="B152" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -20018,7 +20018,7 @@
         <v>296</v>
       </c>
       <c r="B153" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -20026,7 +20026,7 @@
         <v>298</v>
       </c>
       <c r="B154" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -20050,7 +20050,7 @@
         <v>304</v>
       </c>
       <c r="B157" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -20058,7 +20058,7 @@
         <v>308</v>
       </c>
       <c r="B158" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -20066,55 +20066,55 @@
         <v>306</v>
       </c>
       <c r="B159" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B160" t="s">
         <v>1140</v>
-      </c>
-      <c r="B160" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B161" t="s">
         <v>1142</v>
-      </c>
-      <c r="B161" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B162" t="s">
         <v>1144</v>
-      </c>
-      <c r="B162" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B163" t="s">
         <v>1146</v>
-      </c>
-      <c r="B163" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B164" t="s">
         <v>1157</v>
-      </c>
-      <c r="B164" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B165" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>
@@ -20127,8 +20127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20142,7 +20142,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -20150,7 +20150,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -20158,7 +20158,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -20166,7 +20166,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -20174,7 +20174,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -20182,7 +20182,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -20190,7 +20190,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -20198,7 +20198,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -20214,7 +20214,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -20222,7 +20222,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -20230,7 +20230,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -20238,7 +20238,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -20246,7 +20246,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -20254,7 +20254,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -20262,7 +20262,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -20270,7 +20270,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -20278,7 +20278,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -20286,7 +20286,7 @@
         <v>36</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -20294,7 +20294,7 @@
         <v>38</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -20302,7 +20302,7 @@
         <v>40</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -20310,7 +20310,7 @@
         <v>42</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -20318,7 +20318,7 @@
         <v>44</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -20326,7 +20326,7 @@
         <v>46</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -20334,7 +20334,7 @@
         <v>48</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -20342,7 +20342,7 @@
         <v>50</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -20350,7 +20350,7 @@
         <v>52</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -20358,7 +20358,7 @@
         <v>54</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -20366,7 +20366,7 @@
         <v>56</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -20374,7 +20374,7 @@
         <v>58</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -20382,7 +20382,7 @@
         <v>60</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -20390,7 +20390,7 @@
         <v>62</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -20398,7 +20398,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -20406,7 +20406,7 @@
         <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -20414,7 +20414,7 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -20422,7 +20422,7 @@
         <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -20430,7 +20430,7 @@
         <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -20438,7 +20438,7 @@
         <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -20446,7 +20446,7 @@
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -20454,7 +20454,7 @@
         <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -20462,7 +20462,7 @@
         <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -20470,7 +20470,7 @@
         <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -20478,7 +20478,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -20486,7 +20486,7 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -20494,7 +20494,7 @@
         <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -20502,7 +20502,7 @@
         <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -20510,7 +20510,7 @@
         <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -20518,7 +20518,7 @@
         <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -20526,7 +20526,7 @@
         <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -20534,7 +20534,7 @@
         <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -20542,7 +20542,7 @@
         <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -20550,7 +20550,7 @@
         <v>101</v>
       </c>
       <c r="B52" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -20558,7 +20558,7 @@
         <v>103</v>
       </c>
       <c r="B53" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -20566,7 +20566,7 @@
         <v>105</v>
       </c>
       <c r="B54" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -20574,7 +20574,7 @@
         <v>107</v>
       </c>
       <c r="B55" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -20582,7 +20582,7 @@
         <v>109</v>
       </c>
       <c r="B56" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -20590,7 +20590,7 @@
         <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -20598,7 +20598,7 @@
         <v>113</v>
       </c>
       <c r="B58" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -20606,7 +20606,7 @@
         <v>115</v>
       </c>
       <c r="B59" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -20614,7 +20614,7 @@
         <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -20622,7 +20622,7 @@
         <v>119</v>
       </c>
       <c r="B61" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -20630,7 +20630,7 @@
         <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -20638,7 +20638,7 @@
         <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -20646,7 +20646,7 @@
         <v>125</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -20654,7 +20654,7 @@
         <v>127</v>
       </c>
       <c r="B65" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -20662,7 +20662,7 @@
         <v>129</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -20670,7 +20670,7 @@
         <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -20678,7 +20678,7 @@
         <v>133</v>
       </c>
       <c r="B68" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -20686,7 +20686,7 @@
         <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -20694,7 +20694,7 @@
         <v>137</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -20702,7 +20702,7 @@
         <v>139</v>
       </c>
       <c r="B71" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -20710,7 +20710,7 @@
         <v>141</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -20718,7 +20718,7 @@
         <v>143</v>
       </c>
       <c r="B73" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -20726,7 +20726,7 @@
         <v>145</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -20734,7 +20734,7 @@
         <v>147</v>
       </c>
       <c r="B75" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -20742,7 +20742,7 @@
         <v>149</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -20750,7 +20750,7 @@
         <v>151</v>
       </c>
       <c r="B77" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -20758,7 +20758,7 @@
         <v>153</v>
       </c>
       <c r="B78" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -20766,7 +20766,7 @@
         <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -20774,7 +20774,7 @@
         <v>157</v>
       </c>
       <c r="B80" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -20790,7 +20790,7 @@
         <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -20798,7 +20798,7 @@
         <v>24</v>
       </c>
       <c r="B83" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -20806,7 +20806,7 @@
         <v>161</v>
       </c>
       <c r="B84" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -20814,7 +20814,7 @@
         <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -20822,7 +20822,7 @@
         <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -20830,7 +20830,7 @@
         <v>167</v>
       </c>
       <c r="B87" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -20838,7 +20838,7 @@
         <v>169</v>
       </c>
       <c r="B88" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -20846,7 +20846,7 @@
         <v>171</v>
       </c>
       <c r="B89" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -20854,7 +20854,7 @@
         <v>173</v>
       </c>
       <c r="B90" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -20862,7 +20862,7 @@
         <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -20870,7 +20870,7 @@
         <v>177</v>
       </c>
       <c r="B92" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -20878,7 +20878,7 @@
         <v>179</v>
       </c>
       <c r="B93" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -20886,7 +20886,7 @@
         <v>181</v>
       </c>
       <c r="B94" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -20894,7 +20894,7 @@
         <v>183</v>
       </c>
       <c r="B95" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -20902,7 +20902,7 @@
         <v>185</v>
       </c>
       <c r="B96" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -20910,7 +20910,7 @@
         <v>187</v>
       </c>
       <c r="B97" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -20918,7 +20918,7 @@
         <v>189</v>
       </c>
       <c r="B98" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -20926,7 +20926,7 @@
         <v>191</v>
       </c>
       <c r="B99" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -20934,7 +20934,7 @@
         <v>193</v>
       </c>
       <c r="B100" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -20942,7 +20942,7 @@
         <v>195</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -20950,7 +20950,7 @@
         <v>197</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -20958,7 +20958,7 @@
         <v>199</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -20966,7 +20966,7 @@
         <v>201</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -20974,7 +20974,7 @@
         <v>202</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -20982,7 +20982,7 @@
         <v>204</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -20990,7 +20990,7 @@
         <v>206</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -20998,7 +20998,7 @@
         <v>208</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -21006,7 +21006,7 @@
         <v>209</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -21014,7 +21014,7 @@
         <v>211</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -21022,7 +21022,7 @@
         <v>213</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -21030,7 +21030,7 @@
         <v>215</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -21038,7 +21038,7 @@
         <v>216</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -21046,7 +21046,7 @@
         <v>218</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -21054,7 +21054,7 @@
         <v>220</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -21062,7 +21062,7 @@
         <v>222</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -21070,7 +21070,7 @@
         <v>224</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -21078,7 +21078,7 @@
         <v>226</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -21086,7 +21086,7 @@
         <v>228</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -21094,7 +21094,7 @@
         <v>230</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -21102,7 +21102,7 @@
         <v>232</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -21110,7 +21110,7 @@
         <v>234</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -21118,7 +21118,7 @@
         <v>236</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -21126,7 +21126,7 @@
         <v>238</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -21134,7 +21134,7 @@
         <v>240</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -21142,7 +21142,7 @@
         <v>242</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -21150,7 +21150,7 @@
         <v>244</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -21158,7 +21158,7 @@
         <v>246</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -21166,7 +21166,7 @@
         <v>248</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -21174,7 +21174,7 @@
         <v>250</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -21182,7 +21182,7 @@
         <v>252</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -21190,7 +21190,7 @@
         <v>254</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -21198,7 +21198,7 @@
         <v>256</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -21206,7 +21206,7 @@
         <v>258</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -21214,7 +21214,7 @@
         <v>260</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -21222,7 +21222,7 @@
         <v>262</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -21230,7 +21230,7 @@
         <v>264</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -21238,7 +21238,7 @@
         <v>266</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -21254,7 +21254,7 @@
         <v>270</v>
       </c>
       <c r="B140" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -21302,7 +21302,7 @@
         <v>282</v>
       </c>
       <c r="B146" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -21342,7 +21342,7 @@
         <v>292</v>
       </c>
       <c r="B151" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -21350,7 +21350,7 @@
         <v>294</v>
       </c>
       <c r="B152" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -21358,7 +21358,7 @@
         <v>296</v>
       </c>
       <c r="B153" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -21366,7 +21366,7 @@
         <v>298</v>
       </c>
       <c r="B154" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -21390,7 +21390,7 @@
         <v>304</v>
       </c>
       <c r="B157" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -21398,7 +21398,7 @@
         <v>308</v>
       </c>
       <c r="B158" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -21406,55 +21406,55 @@
         <v>306</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B160" t="s">
         <v>1140</v>
-      </c>
-      <c r="B160" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B161" t="s">
         <v>1142</v>
-      </c>
-      <c r="B161" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B162" t="s">
         <v>1144</v>
-      </c>
-      <c r="B162" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B163" t="s">
         <v>1146</v>
-      </c>
-      <c r="B163" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B164" t="s">
         <v>1157</v>
-      </c>
-      <c r="B164" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B165" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>